<commit_message>
cleaned up some code
</commit_message>
<xml_diff>
--- a/project/app/RGB_Hex.xlsx
+++ b/project/app/RGB_Hex.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steph/Desktop/fractal-machine/project/app/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E22FFBC-E905-3D4E-9EF9-8381BD4D0961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="17500" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -853,8 +859,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -917,6 +923,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -963,7 +977,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -995,9 +1009,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1029,6 +1061,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1204,14 +1254,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1281,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1235,7 +1289,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1243,7 +1297,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1251,7 +1305,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1259,7 +1313,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1267,7 +1321,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1275,7 +1329,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1283,7 +1337,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1291,7 +1345,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1299,7 +1353,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1307,7 +1361,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1315,7 +1369,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1323,7 +1377,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1331,7 +1385,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1339,7 +1393,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1347,7 +1401,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1355,7 +1409,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1363,7 +1417,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1371,7 +1425,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1379,7 +1433,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1387,7 +1441,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1395,7 +1449,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1403,7 +1457,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1411,7 +1465,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1419,7 +1473,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1427,7 +1481,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1435,7 +1489,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1443,7 +1497,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1451,7 +1505,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1459,7 +1513,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1467,7 +1521,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1475,7 +1529,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1483,7 +1537,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1491,7 +1545,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1499,7 +1553,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1507,7 +1561,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1515,7 +1569,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1523,7 +1577,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1531,7 +1585,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1539,7 +1593,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1547,7 +1601,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1555,7 +1609,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1563,7 +1617,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1571,7 +1625,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1579,7 +1633,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1587,7 +1641,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1595,7 +1649,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1603,7 +1657,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1611,7 +1665,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1619,7 +1673,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1627,7 +1681,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1635,7 +1689,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1643,7 +1697,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1651,7 +1705,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1659,7 +1713,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1667,7 +1721,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1675,7 +1729,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1683,7 +1737,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1691,7 +1745,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1699,7 +1753,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1707,7 +1761,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1715,7 +1769,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1723,7 +1777,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1731,7 +1785,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1739,7 +1793,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1747,7 +1801,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1755,7 +1809,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1763,7 +1817,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1771,7 +1825,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1779,7 +1833,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -1787,7 +1841,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1795,7 +1849,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -1803,7 +1857,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1811,7 +1865,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1819,7 +1873,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -1827,7 +1881,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -1835,7 +1889,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -1843,7 +1897,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1851,7 +1905,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -1859,7 +1913,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -1867,7 +1921,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -1875,7 +1929,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -1883,7 +1937,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -1891,7 +1945,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -1899,7 +1953,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -1907,7 +1961,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -1915,7 +1969,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -1923,7 +1977,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -1931,7 +1985,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -1939,7 +1993,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -1947,7 +2001,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -1955,7 +2009,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -1963,7 +2017,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -1971,7 +2025,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -1979,7 +2033,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -1987,7 +2041,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -1995,7 +2049,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -2003,7 +2057,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2011,7 +2065,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2019,7 +2073,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2027,7 +2081,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2035,7 +2089,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -2043,7 +2097,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -2051,7 +2105,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -2059,7 +2113,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2067,7 +2121,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2075,7 +2129,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -2083,7 +2137,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2091,7 +2145,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2099,7 +2153,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -2107,7 +2161,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -2115,7 +2169,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -2123,7 +2177,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -2131,7 +2185,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -2139,7 +2193,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -2147,7 +2201,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -2155,7 +2209,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -2163,7 +2217,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -2171,7 +2225,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -2179,7 +2233,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -2187,7 +2241,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -2195,7 +2249,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -2203,7 +2257,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -2211,7 +2265,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -2219,7 +2273,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -2227,7 +2281,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -2235,7 +2289,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -2243,7 +2297,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -2251,7 +2305,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -2259,7 +2313,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -2267,7 +2321,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -2275,7 +2329,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -2283,7 +2337,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -2291,7 +2345,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -2299,7 +2353,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -2307,7 +2361,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -2315,7 +2369,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -2323,7 +2377,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>139</v>
       </c>

</xml_diff>